<commit_message>
minor updates to support more complex loading of data
</commit_message>
<xml_diff>
--- a/template_examples/whole_blood_template.xlsx
+++ b/template_examples/whole_blood_template.xlsx
@@ -1,31 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10512"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27417"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dnunes/cidc-schemas/template_examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlindsay/Documents/Code/cidc/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{674B54B7-4B85-B14A-86D6-EEB824586DDE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1420" yWindow="-17760" windowWidth="27080" windowHeight="14400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-45120" yWindow="2600" windowWidth="45120" windowHeight="23140"/>
   </bookViews>
   <sheets>
     <sheet name="Tissue" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>CIDC</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="B2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -38,7 +45,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="B3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -51,7 +58,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="B4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -64,7 +71,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="B5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -77,7 +84,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+    <comment ref="B6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -90,7 +97,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+    <comment ref="B7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -103,7 +110,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+    <comment ref="B8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -116,7 +123,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+    <comment ref="B9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -129,7 +136,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+    <comment ref="B10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -142,7 +149,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
+    <comment ref="B11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -155,7 +162,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
+    <comment ref="B12" authorId="0">
       <text>
         <r>
           <rPr>
@@ -168,7 +175,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
+    <comment ref="B13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -181,7 +188,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
+    <comment ref="B14" authorId="0">
       <text>
         <r>
           <rPr>
@@ -194,7 +201,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
+    <comment ref="B15" authorId="0">
       <text>
         <r>
           <rPr>
@@ -207,7 +214,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
+    <comment ref="B16" authorId="0">
       <text>
         <r>
           <rPr>
@@ -220,7 +227,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
+    <comment ref="B17" authorId="0">
       <text>
         <r>
           <rPr>
@@ -233,7 +240,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
+    <comment ref="B18" authorId="0">
       <text>
         <r>
           <rPr>
@@ -246,7 +253,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
+    <comment ref="B19" authorId="0">
       <text>
         <r>
           <rPr>
@@ -259,7 +266,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
+    <comment ref="B22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -272,7 +279,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
+    <comment ref="C22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -285,7 +292,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000015000000}">
+    <comment ref="D22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -298,7 +305,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000016000000}">
+    <comment ref="E22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -311,7 +318,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000017000000}">
+    <comment ref="F22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -324,7 +331,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000018000000}">
+    <comment ref="G22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -337,7 +344,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000019000000}">
+    <comment ref="H22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -350,7 +357,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001A000000}">
+    <comment ref="I22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -363,7 +370,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001B000000}">
+    <comment ref="J22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -376,7 +383,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001C000000}">
+    <comment ref="K22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -389,7 +396,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001D000000}">
+    <comment ref="L22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -402,7 +409,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001E000000}">
+    <comment ref="M22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -415,7 +422,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001F000000}">
+    <comment ref="N22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -428,7 +435,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000020000000}">
+    <comment ref="O22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -441,7 +448,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000021000000}">
+    <comment ref="P22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -454,7 +461,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000022000000}">
+    <comment ref="Q22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -467,7 +474,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000023000000}">
+    <comment ref="R22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -480,7 +487,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000024000000}">
+    <comment ref="S22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -493,7 +500,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000025000000}">
+    <comment ref="T22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -506,7 +513,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000026000000}">
+    <comment ref="U22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -519,7 +526,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000027000000}">
+    <comment ref="V22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -537,7 +544,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="75">
   <si>
     <t>#t</t>
   </si>
@@ -735,12 +742,39 @@
   </si>
   <si>
     <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>P888</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -906,9 +940,9 @@
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -936,31 +970,14 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -988,23 +1005,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1180,11 +1180,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V222"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1221,7 +1221,7 @@
       <c r="U1" s="5"/>
       <c r="V1" s="5"/>
     </row>
-    <row r="2" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1251,7 +1251,7 @@
       <c r="U2" s="1"/>
       <c r="V2" s="1"/>
     </row>
-    <row r="3" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1281,7 +1281,7 @@
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
     </row>
-    <row r="4" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1311,7 +1311,7 @@
       <c r="U4" s="1"/>
       <c r="V4" s="1"/>
     </row>
-    <row r="5" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1341,7 +1341,7 @@
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
     </row>
-    <row r="6" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1371,7 +1371,7 @@
       <c r="U6" s="1"/>
       <c r="V6" s="1"/>
     </row>
-    <row r="7" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1401,7 +1401,7 @@
       <c r="U7" s="1"/>
       <c r="V7" s="1"/>
     </row>
-    <row r="8" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -1431,7 +1431,7 @@
       <c r="U8" s="1"/>
       <c r="V8" s="1"/>
     </row>
-    <row r="9" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -1461,7 +1461,7 @@
       <c r="U9" s="1"/>
       <c r="V9" s="1"/>
     </row>
-    <row r="10" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1491,7 +1491,7 @@
       <c r="U10" s="1"/>
       <c r="V10" s="1"/>
     </row>
-    <row r="11" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -1521,7 +1521,7 @@
       <c r="U11" s="1"/>
       <c r="V11" s="1"/>
     </row>
-    <row r="12" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -1551,7 +1551,7 @@
       <c r="U12" s="1"/>
       <c r="V12" s="1"/>
     </row>
-    <row r="13" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -1581,7 +1581,7 @@
       <c r="U13" s="1"/>
       <c r="V13" s="1"/>
     </row>
-    <row r="14" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -1611,7 +1611,7 @@
       <c r="U14" s="1"/>
       <c r="V14" s="1"/>
     </row>
-    <row r="15" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -1641,7 +1641,7 @@
       <c r="U15" s="1"/>
       <c r="V15" s="1"/>
     </row>
-    <row r="16" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -1671,7 +1671,7 @@
       <c r="U16" s="1"/>
       <c r="V16" s="1"/>
     </row>
-    <row r="17" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -1701,7 +1701,7 @@
       <c r="U17" s="1"/>
       <c r="V17" s="1"/>
     </row>
-    <row r="18" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -1731,7 +1731,7 @@
       <c r="U18" s="1"/>
       <c r="V18" s="1"/>
     </row>
-    <row r="19" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -1866,8 +1866,8 @@
       <c r="C23">
         <v>54321</v>
       </c>
-      <c r="D23">
-        <v>12345</v>
+      <c r="D23" t="s">
+        <v>72</v>
       </c>
       <c r="E23">
         <v>54321</v>
@@ -1878,8 +1878,8 @@
       <c r="G23">
         <v>54321</v>
       </c>
-      <c r="H23">
-        <v>12345</v>
+      <c r="H23" t="s">
+        <v>69</v>
       </c>
       <c r="I23" s="4" t="s">
         <v>54</v>
@@ -1905,8 +1905,8 @@
       <c r="P23" t="s">
         <v>60</v>
       </c>
-      <c r="Q23">
-        <v>12344</v>
+      <c r="Q23" t="s">
+        <v>55</v>
       </c>
       <c r="R23">
         <v>500</v>
@@ -1934,8 +1934,8 @@
       <c r="C24">
         <v>54321</v>
       </c>
-      <c r="D24">
-        <v>12345</v>
+      <c r="D24" t="s">
+        <v>74</v>
       </c>
       <c r="E24">
         <v>54321</v>
@@ -1946,8 +1946,8 @@
       <c r="G24">
         <v>54321</v>
       </c>
-      <c r="H24">
-        <v>12345</v>
+      <c r="H24" t="s">
+        <v>69</v>
       </c>
       <c r="I24" s="4" t="s">
         <v>54</v>
@@ -1973,8 +1973,8 @@
       <c r="P24" t="s">
         <v>60</v>
       </c>
-      <c r="Q24">
-        <v>12344</v>
+      <c r="Q24" t="s">
+        <v>64</v>
       </c>
       <c r="R24">
         <v>500</v>
@@ -2002,8 +2002,8 @@
       <c r="C25">
         <v>54321</v>
       </c>
-      <c r="D25">
-        <v>12345</v>
+      <c r="D25" t="s">
+        <v>72</v>
       </c>
       <c r="E25">
         <v>54321</v>
@@ -2014,8 +2014,8 @@
       <c r="G25">
         <v>54321</v>
       </c>
-      <c r="H25">
-        <v>12345</v>
+      <c r="H25" t="s">
+        <v>70</v>
       </c>
       <c r="I25" s="4" t="s">
         <v>54</v>
@@ -2041,8 +2041,8 @@
       <c r="P25" t="s">
         <v>60</v>
       </c>
-      <c r="Q25">
-        <v>12344</v>
+      <c r="Q25" t="s">
+        <v>65</v>
       </c>
       <c r="R25">
         <v>500</v>
@@ -2070,8 +2070,8 @@
       <c r="C26">
         <v>54321</v>
       </c>
-      <c r="D26">
-        <v>12345</v>
+      <c r="D26" t="s">
+        <v>72</v>
       </c>
       <c r="E26">
         <v>54321</v>
@@ -2082,8 +2082,8 @@
       <c r="G26">
         <v>54321</v>
       </c>
-      <c r="H26">
-        <v>12345</v>
+      <c r="H26" t="s">
+        <v>70</v>
       </c>
       <c r="I26" s="4" t="s">
         <v>54</v>
@@ -2109,8 +2109,8 @@
       <c r="P26" t="s">
         <v>60</v>
       </c>
-      <c r="Q26">
-        <v>12344</v>
+      <c r="Q26" t="s">
+        <v>66</v>
       </c>
       <c r="R26">
         <v>500</v>
@@ -2138,8 +2138,8 @@
       <c r="C27">
         <v>54321</v>
       </c>
-      <c r="D27">
-        <v>12345</v>
+      <c r="D27" t="s">
+        <v>73</v>
       </c>
       <c r="E27">
         <v>54321</v>
@@ -2150,8 +2150,8 @@
       <c r="G27">
         <v>54321</v>
       </c>
-      <c r="H27">
-        <v>12345</v>
+      <c r="H27" t="s">
+        <v>71</v>
       </c>
       <c r="I27" s="4" t="s">
         <v>54</v>
@@ -2177,8 +2177,8 @@
       <c r="P27" t="s">
         <v>60</v>
       </c>
-      <c r="Q27">
-        <v>12344</v>
+      <c r="Q27" t="s">
+        <v>67</v>
       </c>
       <c r="R27">
         <v>500</v>
@@ -2206,8 +2206,8 @@
       <c r="C28">
         <v>54321</v>
       </c>
-      <c r="D28">
-        <v>12345</v>
+      <c r="D28" t="s">
+        <v>73</v>
       </c>
       <c r="E28">
         <v>54321</v>
@@ -2218,8 +2218,8 @@
       <c r="G28">
         <v>54321</v>
       </c>
-      <c r="H28">
-        <v>12345</v>
+      <c r="H28" t="s">
+        <v>71</v>
       </c>
       <c r="I28" s="4" t="s">
         <v>54</v>
@@ -2245,8 +2245,8 @@
       <c r="P28" t="s">
         <v>60</v>
       </c>
-      <c r="Q28">
-        <v>12344</v>
+      <c r="Q28" t="s">
+        <v>68</v>
       </c>
       <c r="R28">
         <v>500</v>
@@ -3241,37 +3241,37 @@
     <mergeCell ref="Q21:V21"/>
   </mergeCells>
   <dataValidations count="11">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5">
       <formula1>"Assay-1,Assay-2,Assay-3,Assay-4,Assay-5,Assay-6,Assay-7,Assay-8,Assay-9,Assay-10,Assay-11,Assay-12,Assay-13,Assay-14,Assay-15,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10">
       <formula1>"FEDEX,USPS,UPC"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13">
       <formula1>"Frozen (Dry Ice),Frozen (Dry Shipper),Ambient (Ice Pack),Ambient,Other"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="C14" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="C14">
       <formula1>AND(ISNUMBER(C14),LEFT(CELL("format",C14),1)="D")</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K23:K222" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K23:K222">
       <formula1>"Core Needle Biopsy,Surgical Resection,Endoscopic Biopsy,Punch Biopsy,Plasma,PBMC,Whole Blood,Stool Sample,Bone Marrow Aspirate,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L23:L222" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L23:L222">
       <formula1>"FFPE Block,FFPE Scroll,FFPE Core Punch,Unstained Slide,Frozen Tissue,Sodium Heparin Green-Top Tube,Streck Tube,EDTA Tube,Archival FFPE Block,Archival FFPE Slides,Archival FFPE Core Punch,Archival FFPE Scroll,Frozen Stool,DNA-Preserved Stool,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M23:M222" xr:uid="{00000000-0002-0000-0000-000006000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M23:M222">
       <formula1>"DNA,RNA,cfDNA,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O23:O222" xr:uid="{00000000-0002-0000-0000-000007000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O23:O222">
       <formula1>"µL,mL,mg,ng,Vials,Slides,Scrolls,Blocks,ng/µL,cells/ml,N/A,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T23:T222" xr:uid="{00000000-0002-0000-0000-000008000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T23:T222">
       <formula1>"Usable for Assay,Not Usable for Assay,Verifying,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U23:U222" xr:uid="{00000000-0002-0000-0000-000009000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U23:U222">
       <formula1>"Replacement Requested,Replacement Tested,N/A"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V23:V222" xr:uid="{00000000-0002-0000-0000-00000A000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V23:V222">
       <formula1>"Sample Returned,Sample Exhausted,Remainder used for other Assay,Other,Sample Leftover"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>